<commit_message>
added notes from call with armando
</commit_message>
<xml_diff>
--- a/Popular Courses.xlsx
+++ b/Popular Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfreestone\Code\athsrueas\geo_bounties\AI_courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1713A54C-2188-4B80-B548-A41029A054C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F158C4E3-388A-48D8-8B3C-9841684840F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
@@ -1062,18 +1062,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="123.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DAE171-A70F-45DD-8FAD-078A6DA22C65}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>

</xml_diff>